<commit_message>
minor changes results for round 4
</commit_message>
<xml_diff>
--- a/part_3_cohere/analysis/Round_4_scibert/dense_answer_relevance_results_jats.xlsx
+++ b/part_3_cohere/analysis/Round_4_scibert/dense_answer_relevance_results_jats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/poppyriddle/Documents/PhD/Research_proposal/Part_3/part_3_cohere/analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/poppyriddle/Documents/Github/Research_proposal/part_3_cohere/analysis/Round_4_scibert/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC38C23-555A-7A49-8DE4-A6C080177999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B437FFA6-E0D6-EB4A-9573-3E1AF3773930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37400" yWindow="500" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw data" sheetId="1" r:id="rId1"/>

</xml_diff>